<commit_message>
update vkct terminy 2025
</commit_message>
<xml_diff>
--- a/2025/01-brumov/01-VKCT2025-Brumov.xlsx
+++ b/2025/01-brumov/01-VKCT2025-Brumov.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Předškoláci I" sheetId="1" state="visible" r:id="rId3"/>
@@ -4511,7 +4511,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5606,8 +5606,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5703,8 +5703,8 @@
       <c r="C5" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>2007</v>
+      <c r="D5" s="11" t="n">
+        <v>2008</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>393</v>
@@ -10602,7 +10602,7 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>